<commit_message>
date doesn't work yet will work on that later
</commit_message>
<xml_diff>
--- a/ExportedFiles/excelFiles/monitor_availability.xlsx
+++ b/ExportedFiles/excelFiles/monitor_availability.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,6 +721,174 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:12:14</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>monitor_availability</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label-wrapper button[aria-label*='10-01']"}
+  (Session info: chrome=128.0.6613.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF7F082B5D2+29090]
+	(No symbol) [0x00007FF7F079E689]
+	(No symbol) [0x00007FF7F065B1CA]
+	(No symbol) [0x00007FF7F06AEFD7]
+	(No symbol) [0x00007FF7F06AF22C]
+	(No symbol) [0x00007FF7F06F97F7]
+	(No symbol) [0x00007FF7F06D672F]
+	(No symbol) [0x00007FF7F06F65D9]
+	(No symbol) [0x00007FF7F06D6493]
+	(No symbol) [0x00007FF7F06A09B1]
+	(No symbol) [0x00007FF7F06A1B11]
+	GetHandleVerifier [0x00007FF7F0B48C5D+3295277]
+	GetHandleVerifier [0x00007FF7F0B94843+3605523]
+	GetHandleVerifier [0x00007FF7F0B8A707+3564247]
+	GetHandleVerifier [0x00007FF7F08E6EB6+797318]
+	(No symbol) [0x00007FF7F07A980F]
+	(No symbol) [0x00007FF7F07A53F4]
+	(No symbol) [0x00007FF7F07A5580]
+	(No symbol) [0x00007FF7F0794A1F]
+	BaseThreadInitThunk [0x00007FFC979C257D+29]
+	RtlUserThreadStart [0x00007FFC9896AF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>17:12:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:12:35</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>monitor_availability</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label-wrapper button[aria-label*='10-01']"}
+  (Session info: chrome=128.0.6613.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF7F082B5D2+29090]
+	(No symbol) [0x00007FF7F079E689]
+	(No symbol) [0x00007FF7F065B1CA]
+	(No symbol) [0x00007FF7F06AEFD7]
+	(No symbol) [0x00007FF7F06AF22C]
+	(No symbol) [0x00007FF7F06F97F7]
+	(No symbol) [0x00007FF7F06D672F]
+	(No symbol) [0x00007FF7F06F65D9]
+	(No symbol) [0x00007FF7F06D6493]
+	(No symbol) [0x00007FF7F06A09B1]
+	(No symbol) [0x00007FF7F06A1B11]
+	GetHandleVerifier [0x00007FF7F0B48C5D+3295277]
+	GetHandleVerifier [0x00007FF7F0B94843+3605523]
+	GetHandleVerifier [0x00007FF7F0B8A707+3564247]
+	GetHandleVerifier [0x00007FF7F08E6EB6+797318]
+	(No symbol) [0x00007FF7F07A980F]
+	(No symbol) [0x00007FF7F07A53F4]
+	(No symbol) [0x00007FF7F07A5580]
+	(No symbol) [0x00007FF7F0794A1F]
+	BaseThreadInitThunk [0x00007FFC979C257D+29]
+	RtlUserThreadStart [0x00007FFC9896AF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>17:12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-09-09 17:12:56</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>monitor_availability</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.opentable.com/r/bar-spero-washington/</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Failed to select the date: Message: no such element: Unable to locate element: {"method":"css selector","selector":"#restProfileSideBarDtpDayPicker-label-wrapper button[aria-label*='10-01']"}
+  (Session info: chrome=128.0.6613.120); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
+Stacktrace:
+	GetHandleVerifier [0x00007FF7F082B5D2+29090]
+	(No symbol) [0x00007FF7F079E689]
+	(No symbol) [0x00007FF7F065B1CA]
+	(No symbol) [0x00007FF7F06AEFD7]
+	(No symbol) [0x00007FF7F06AF22C]
+	(No symbol) [0x00007FF7F06F97F7]
+	(No symbol) [0x00007FF7F06D672F]
+	(No symbol) [0x00007FF7F06F65D9]
+	(No symbol) [0x00007FF7F06D6493]
+	(No symbol) [0x00007FF7F06A09B1]
+	(No symbol) [0x00007FF7F06A1B11]
+	GetHandleVerifier [0x00007FF7F0B48C5D+3295277]
+	GetHandleVerifier [0x00007FF7F0B94843+3605523]
+	GetHandleVerifier [0x00007FF7F0B8A707+3564247]
+	GetHandleVerifier [0x00007FF7F08E6EB6+797318]
+	(No symbol) [0x00007FF7F07A980F]
+	(No symbol) [0x00007FF7F07A53F4]
+	(No symbol) [0x00007FF7F07A5580]
+	(No symbol) [0x00007FF7F0794A1F]
+	BaseThreadInitThunk [0x00007FFC979C257D+29]
+	RtlUserThreadStart [0x00007FFC9896AF28+40]
+</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2024-09-09</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>17:12:56</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>